<commit_message>
Revert "Revert "Reproducable Results""
This reverts commit 696922c2efd493718cb66d96a205d13e1d50a74b.
</commit_message>
<xml_diff>
--- a/smart_search/Prady_Status_Report.xlsx
+++ b/smart_search/Prady_Status_Report.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\MedIX_Project\smart_search\"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,6 +1374,15 @@
       <c r="C9" s="15" t="s">
         <v>82</v>
       </c>
+      <c r="D9" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
@@ -1385,6 +1394,15 @@
       <c r="C10" s="15" t="s">
         <v>83</v>
       </c>
+      <c r="D10" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
@@ -1396,6 +1414,15 @@
       <c r="C11" s="15" t="s">
         <v>84</v>
       </c>
+      <c r="D11" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
@@ -1406,6 +1433,15 @@
       </c>
       <c r="C12" s="15" t="s">
         <v>85</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1836,7 +1872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1874,9 +1912,15 @@
       <c r="C2" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="D2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
@@ -1888,9 +1932,15 @@
       <c r="C3" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="D3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
@@ -1902,9 +1952,15 @@
       <c r="C4" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="D4" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
@@ -1916,9 +1972,15 @@
       <c r="C5" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="D5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
@@ -1930,7 +1992,9 @@
       <c r="C6" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
     </row>

</xml_diff>